<commit_message>
alterando dados para facilitar o mobile
</commit_message>
<xml_diff>
--- a/Banco/Importar/Modelo_de_dados.xlsx
+++ b/Banco/Importar/Modelo_de_dados.xlsx
@@ -5,19 +5,21 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51963902866\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\51963902866\Documents\projetos\MedicalGroup-master\Banco\Importar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Especialidade" sheetId="2" r:id="rId1"/>
     <sheet name="Clinica" sheetId="7" r:id="rId2"/>
-    <sheet name="Medico" sheetId="3" r:id="rId3"/>
-    <sheet name="Paciente" sheetId="4" r:id="rId4"/>
-    <sheet name="Usuario" sheetId="6" r:id="rId5"/>
-    <sheet name="Consulta" sheetId="5" r:id="rId6"/>
+    <sheet name="Tipo Usuario" sheetId="8" r:id="rId3"/>
+    <sheet name="Usuario" sheetId="9" r:id="rId4"/>
+    <sheet name="Medico" sheetId="10" r:id="rId5"/>
+    <sheet name="status consulta" sheetId="11" r:id="rId6"/>
+    <sheet name="Paciente" sheetId="4" r:id="rId7"/>
+    <sheet name="Consulta" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>SP Medical Group</t>
   </si>
@@ -202,9 +204,6 @@
     <t>Av. Barão Limeira</t>
   </si>
   <si>
-    <t>ID Usuario</t>
-  </si>
-  <si>
     <t>ID_Usuario</t>
   </si>
   <si>
@@ -229,17 +228,44 @@
     <t>NOME FANTASIA</t>
   </si>
   <si>
-    <t>endereco</t>
-  </si>
-  <si>
-    <t>?????</t>
+    <t>med132</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Agendada</t>
+  </si>
+  <si>
+    <t>Realizada</t>
+  </si>
+  <si>
+    <t>Cancelada</t>
+  </si>
+  <si>
+    <t>ID_Usuarios</t>
+  </si>
+  <si>
+    <t>Endereco</t>
+  </si>
+  <si>
+    <t>????</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,14 +327,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -331,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -344,7 +362,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -750,16 +767,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
@@ -784,87 +801,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="19.6640625" style="2"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>10</v>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -874,379 +837,519 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="3"/>
-    <col min="2" max="2" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="23.44140625" style="3"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>27</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="8">
-        <v>30602</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1134567654</v>
-      </c>
-      <c r="D2" s="3">
-        <v>435225435</v>
-      </c>
-      <c r="E2" s="3">
-        <v>94839859000</v>
-      </c>
-      <c r="F2" s="3">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="8">
-        <v>37095</v>
-      </c>
-      <c r="C3" s="3">
-        <v>11987656543</v>
-      </c>
-      <c r="D3" s="3">
-        <v>326543457</v>
-      </c>
-      <c r="E3" s="3">
-        <v>73556944057</v>
-      </c>
-      <c r="F3" s="3">
+      <c r="B2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="8">
-        <v>28773</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1197204453</v>
-      </c>
-      <c r="D4" s="3">
-        <v>546365253</v>
-      </c>
-      <c r="E4" s="3">
-        <v>16839338002</v>
-      </c>
-      <c r="F4" s="3">
+      <c r="C2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="8">
-        <v>31333</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1134566543</v>
-      </c>
-      <c r="D5" s="3">
-        <v>543663625</v>
-      </c>
-      <c r="E5" s="3">
-        <v>14332654765</v>
-      </c>
-      <c r="F5" s="3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="8">
-        <v>27633</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1176566377</v>
-      </c>
-      <c r="D6" s="3">
-        <v>325444441</v>
-      </c>
-      <c r="E6" s="3">
-        <v>91305348010</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="8">
-        <v>26379</v>
-      </c>
-      <c r="C7" s="3">
-        <v>11954368769</v>
-      </c>
-      <c r="D7" s="3">
-        <v>545662667</v>
-      </c>
-      <c r="E7" s="3">
-        <v>79799299004</v>
-      </c>
-      <c r="F7" s="3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="8">
-        <v>43164</v>
-      </c>
-      <c r="C8" s="3">
-        <v>11969584932</v>
-      </c>
-      <c r="D8" s="3">
-        <v>545662668</v>
-      </c>
-      <c r="E8" s="3">
-        <v>13771913039</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C8" r:id="rId1"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId7"/>
+    <hyperlink ref="C11" r:id="rId8"/>
+    <hyperlink ref="C10" r:id="rId9"/>
+    <hyperlink ref="C9" r:id="rId10"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4">
+      <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J16" s="12"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1"/>
-    <hyperlink ref="A7" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="A3" r:id="rId6"/>
-    <hyperlink ref="A2" r:id="rId7"/>
-    <hyperlink ref="A11" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A9" r:id="rId10"/>
-  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="23.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="23.44140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3">
+        <v>435225435</v>
+      </c>
+      <c r="D2" s="3">
+        <v>94839859000</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="8">
+        <v>30602</v>
+      </c>
+      <c r="G2" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="3">
+        <v>326543457</v>
+      </c>
+      <c r="D3" s="3">
+        <v>73556944057</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="8">
+        <v>37095</v>
+      </c>
+      <c r="G3" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3">
+        <v>546365253</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16839338002</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="8">
+        <v>28773</v>
+      </c>
+      <c r="G4" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3">
+        <v>543663625</v>
+      </c>
+      <c r="D5" s="3">
+        <v>14332654765</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="8">
+        <v>31333</v>
+      </c>
+      <c r="G5" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3">
+        <v>325444441</v>
+      </c>
+      <c r="D6" s="3">
+        <v>91305348010</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="8">
+        <v>27633</v>
+      </c>
+      <c r="G6" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3">
+        <v>545662667</v>
+      </c>
+      <c r="D7" s="3">
+        <v>79799299004</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="8">
+        <v>26379</v>
+      </c>
+      <c r="G7" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3">
+        <v>545662668</v>
+      </c>
+      <c r="D8" s="3">
+        <v>13771913039</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="8">
+        <v>43164</v>
+      </c>
+      <c r="G8" s="3">
+        <v>11967485322</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -1278,7 +1381,7 @@
         <v>45</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1295,7 +1398,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,7 +1415,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1329,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,7 +1449,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1363,7 +1466,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1380,7 +1483,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1397,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>